<commit_message>
new dp medium problem
</commit_message>
<xml_diff>
--- a/pattern.xlsx
+++ b/pattern.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Learning\LeetCode-Javascript-Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B92163C-3C96-4593-BD8D-741E674EF0DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F903B8DF-9399-4E40-89C5-D31676DD389A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Maximum SubArray</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Leetcode - 51</t>
   </si>
@@ -40,6 +37,18 @@
   </si>
   <si>
     <t>Leetcode - 718</t>
+  </si>
+  <si>
+    <t>DP on Matrix</t>
+  </si>
+  <si>
+    <t>Leetcode - 200</t>
+  </si>
+  <si>
+    <t>Leetcode - 221</t>
+  </si>
+  <si>
+    <t>Maximum/Minimum SubArray</t>
   </si>
 </sst>
 </file>
@@ -366,37 +375,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
+      <c r="E3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new dp medium problems
</commit_message>
<xml_diff>
--- a/pattern.xlsx
+++ b/pattern.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Learning\LeetCode-Javascript-Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F903B8DF-9399-4E40-89C5-D31676DD389A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EAA468-351E-4157-8807-B1817C6B6E3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Leetcode - 51</t>
   </si>
@@ -49,6 +49,21 @@
   </si>
   <si>
     <t>Maximum/Minimum SubArray</t>
+  </si>
+  <si>
+    <t>House Robber Pattern</t>
+  </si>
+  <si>
+    <t>Leetcode - 198</t>
+  </si>
+  <si>
+    <t>Leetcode - 740</t>
+  </si>
+  <si>
+    <t>Stock Graph Pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leetcode - 45 </t>
   </si>
 </sst>
 </file>
@@ -375,20 +390,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -398,8 +415,14 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -409,13 +432,22 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>